<commit_message>
simulator img updated in 230606
</commit_message>
<xml_diff>
--- a/flask_excel.xlsx
+++ b/flask_excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\황지혁\Desktop\MRMR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4253D8A-37F4-481E-BE20-EDFF64CF438C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E78F7F85-BCC8-4D60-87E4-7F408DF08382}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{680BF0FC-A31B-4061-9FEF-D77DD519C956}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>1stCar</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -107,6 +107,10 @@
   </si>
   <si>
     <t>bus22</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bus3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -473,8 +477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{580A4239-145A-4FED-8449-917AF067D060}">
   <dimension ref="A1:H1253"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -710,6 +714,27 @@
       <c r="A26">
         <v>25</v>
       </c>
+      <c r="B26" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26">
+        <v>15</v>
+      </c>
+      <c r="D26" t="s">
+        <v>14</v>
+      </c>
+      <c r="E26">
+        <v>18</v>
+      </c>
+      <c r="F26" t="s">
+        <v>15</v>
+      </c>
+      <c r="G26">
+        <v>51</v>
+      </c>
+      <c r="H26">
+        <v>60</v>
+      </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A27">

</xml_diff>